<commit_message>
Delete Spring Security Dependency
</commit_message>
<xml_diff>
--- a/ProjectSpec.xlsx
+++ b/ProjectSpec.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -32,10 +32,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>addinfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>추가정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -48,51 +44,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>사용자정보 입력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자정보 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자정보 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자정보 삭제(탈퇴)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인증로직</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 이메일 + 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소셜로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스프링시큐리티?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포트폴리오 생성로직</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화면 Tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 로그인 이메일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2. 추가정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화면별 개발사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-화면 소개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 소셜로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 사용자정보 입력, 수정, 조회, 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 자기소개, 기술경력 등등 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포트폴리오 양식 고르는 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>portfolio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고른 양식에 사용자정보 값 불러와서 채워넣어줌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PDF 출력 가능하도록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -100,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,16 +127,31 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -176,22 +203,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -215,13 +306,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>480060</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
@@ -262,13 +353,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>472440</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -309,13 +400,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>563880</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
@@ -356,13 +447,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>198120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
@@ -403,13 +494,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>198120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>548640</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>198120</xdr:rowOff>
@@ -450,13 +541,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>624840</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
@@ -497,13 +588,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>327660</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
@@ -832,135 +923,448 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O25"/>
+  <dimension ref="B1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.296875" customWidth="1"/>
+    <col min="1" max="2" width="3.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B1" t="s">
+    <row r="1" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="P2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="17"/>
+    </row>
+    <row r="3" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="9"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="20"/>
+    </row>
+    <row r="4" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="5"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9"/>
+      <c r="P4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B5" s="5"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
+      <c r="P5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B6" s="5"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B7" s="5"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
+      <c r="P7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="9"/>
+      <c r="P8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="9"/>
+      <c r="P10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B11" s="5"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
+      <c r="P11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B12" s="5"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="P12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="O2" t="s">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B13" s="5"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="9"/>
+      <c r="P14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="5"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="9"/>
+      <c r="P15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B16" s="5"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="5"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="O3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="4"/>
-      <c r="O4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="O5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="O7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="O8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="G9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="O9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="O10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="O12" t="s">
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
+      <c r="P17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B18" s="5"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
+      <c r="P18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B19" s="5"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
+      <c r="P19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B20" s="5"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B21" s="5"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B22" s="5"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="5"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B24" s="5"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="D16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="G17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.4">
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.4">
-      <c r="D24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="5"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="9"/>
+    </row>
+    <row r="26" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="D24:E25"/>
+  <mergeCells count="7">
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="P2:U3"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="H9:I10"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="E16:F17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>